<commit_message>
Fix Table & Loc, can run in android
</commit_message>
<xml_diff>
--- a/Designer/Excel/Loc.xlsx
+++ b/Designer/Excel/Loc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fancyHub\UnityLibs\Designer\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71DCAB1-003F-4896-86B6-591B5B02B5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224D783E-8445-44E8-9402-63DD092111D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>TC_VAL_TC_A</t>
   </si>
@@ -109,11 +109,19 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Assets/Res/UI/Sprite/icon.png</t>
+    <t>Assets/Res/UI/Sprite/s2.png</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Assets/Res/UI/Sprite/btn_press.png</t>
+    <t>Assets/Res/UI/Sprite/s1.png</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCIMAGE_VAL_TEXTUREA</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Assets/Res/UI/Texture/t2.png</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -763,7 +771,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1081,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1225,15 +1240,31 @@
         <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>27</v>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A1:S1 A3:S3 B4:B11">
+  <conditionalFormatting sqref="A1:S1 A3:S3 B4:B12">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>公式单元格=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>公式单元格=TRUE</formula>
     </cfRule>

</xml_diff>